<commit_message>
update source index + fix age group
</commit_message>
<xml_diff>
--- a/data/source_index.xlsx
+++ b/data/source_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qleclerc\Documents\R\vivli2024\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leclercq\Documents\R\vivli2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7149448-218D-4BE2-8716-5F5434426347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C351E4A-5C6D-4D3A-B7AB-A6B0D878F408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11950" yWindow="740" windowWidth="25800" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
   <si>
     <t>How to read: if the string in "contains" is found in the raw data, the source is converted to the corresponding value is "match"</t>
   </si>
@@ -361,7 +361,25 @@
     <t>other</t>
   </si>
   <si>
-    <t>SST</t>
+    <t>ovary</t>
+  </si>
+  <si>
+    <t>vomit</t>
+  </si>
+  <si>
+    <t>ascetic fluid</t>
+  </si>
+  <si>
+    <t>ileum</t>
+  </si>
+  <si>
+    <t>paracentesis fluid</t>
+  </si>
+  <si>
+    <t>spleen</t>
+  </si>
+  <si>
+    <t>too vague?</t>
   </si>
 </sst>
 </file>
@@ -656,25 +674,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -685,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="50.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -696,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -705,7 +723,7 @@
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -716,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -725,7 +743,7 @@
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -734,7 +752,7 @@
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -743,7 +761,7 @@
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -752,7 +770,7 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -761,7 +779,7 @@
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -770,7 +788,7 @@
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>
@@ -779,7 +797,7 @@
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -788,7 +806,7 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -797,7 +815,7 @@
       </c>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
@@ -806,7 +824,7 @@
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -815,7 +833,7 @@
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -824,723 +842,764 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="38" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="B40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="B44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="B50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="B51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="B52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="3"/>
-    </row>
-    <row r="54" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="3"/>
-    </row>
-    <row r="55" spans="1:3" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="3"/>
-    </row>
-    <row r="57" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" ht="75.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C59" s="3"/>
-    </row>
-    <row r="60" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="B64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="B65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="B66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C62" s="3"/>
-    </row>
-    <row r="63" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="B67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C63" s="3"/>
-    </row>
-    <row r="64" spans="1:3" ht="90" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="B68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" ht="88" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="B69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="70" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="B70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="B71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="B72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C68" s="3"/>
-    </row>
-    <row r="69" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="B73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="B74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C70" s="3"/>
-    </row>
-    <row r="71" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C77" s="3"/>
-    </row>
-    <row r="78" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C79" s="3"/>
-    </row>
-    <row r="80" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C80" s="3"/>
-    </row>
-    <row r="81" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C81" s="3"/>
-    </row>
-    <row r="82" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C85" s="3"/>
-    </row>
-    <row r="86" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C89" s="3"/>
-    </row>
-    <row r="90" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C91" s="3"/>
-    </row>
-    <row r="92" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C92" s="3"/>
-    </row>
-    <row r="93" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C93" s="3"/>
-    </row>
-    <row r="94" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97" spans="1:3" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B99" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B100" s="3" t="s">
         <v>99</v>
+      </c>
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>